<commit_message>
not bad right now
</commit_message>
<xml_diff>
--- a/Berufsprofile-Kompetenzraster.xlsx
+++ b/Berufsprofile-Kompetenzraster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielschmocker/Documents/Projekte/Benjamin/Berufsprofile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCFE0BE-0471-8947-B898-709F00C5973D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFAFB02-D263-2046-AC80-6319EDB245A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompetenzraster" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="203">
   <si>
     <t>lable</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>funktionale und statistische Zusammenhänge erforschen, dazu Fragen stellen sowie Ergebnisse vergleichen</t>
+  </si>
+  <si>
+    <t>DetailhandelsassistentIn EBA</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F122"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4879,7 +4882,7 @@
         <v>94</v>
       </c>
       <c r="C79" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D79" t="str">
         <f>B79&amp;M79</f>
@@ -4928,7 +4931,7 @@
         <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D80" t="str">
         <f>B80&amp;M80</f>
@@ -4977,7 +4980,7 @@
         <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D81" t="str">
         <f>B81&amp;M81</f>
@@ -5026,7 +5029,7 @@
         <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D82" t="str">
         <f>B82&amp;M82</f>
@@ -5075,7 +5078,7 @@
         <v>94</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D83" t="str">
         <f>B83&amp;M83</f>
@@ -5124,7 +5127,7 @@
         <v>94</v>
       </c>
       <c r="C84" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D84" t="str">
         <f>B84&amp;M84</f>
@@ -5173,7 +5176,7 @@
         <v>94</v>
       </c>
       <c r="C85" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D85" t="str">
         <f>B85&amp;M85</f>
@@ -7035,20 +7038,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8200FB-305B-E64F-B9C4-B1DA92FAD6FD}">
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7058,8 +7061,11 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>Kompetenzraster!G2</f>
         <v>Grundoperationen mit natürlichen Zahlen durchführen</v>
@@ -7071,8 +7077,11 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>Kompetenzraster!G3</f>
         <v>Zahlen erkennen, die durch 2, 5, 10, 100, 1'000 teibar sind</v>
@@ -7084,8 +7093,11 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Kompetenzraster!G4</f>
         <v>Zahlen bis 1 Milliarde lesen udn schreiben</v>
@@ -7097,8 +7109,11 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Kompetenzraster!G5</f>
         <v>Grundoperationen mit natürlichen Zahlen überschlagen</v>
@@ -7107,8 +7122,11 @@
         <f>Kompetenzraster!H5</f>
         <v>ZuVGaZ1.1.1B2_desc</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Kompetenzraster!G6</f>
         <v>Teilbarkeitsregeln (3,4,6,8,9,25,50) nutzen und Teiler natürlicher Zahlen bestimmen</v>
@@ -7118,7 +7136,7 @@
         <v>ZuVGaZ1.1.1C1_desc</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>Kompetenzraster!G7</f>
         <v>Grundoperationnen mit ganzen Zahlen durchführen</v>
@@ -7128,7 +7146,7 @@
         <v>ZuVGaZ1.1.1D1_desc</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Kompetenzraster!G8</f>
         <v>natürliche Zahlen in Primfaktoren zerlegen</v>
@@ -7138,7 +7156,7 @@
         <v>ZuVGaZ1.1.1E1_desc</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>Kompetenzraster!G9</f>
         <v>Die ersten 20 Quadratzahlen ohne TR bestimmen und geometrisch deuten</v>
@@ -7150,8 +7168,11 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Kompetenzraster!G10</f>
         <v>Wurzeln und Potenzen mit dem Rechner berechnen, sowie einfache Wurzeln unt Potenzen im Kopf bestimmen</v>
@@ -7161,7 +7182,7 @@
         <v>ZuVGaZ1.1.2B1_desc</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Kompetenzraster!G11</f>
         <v>Ein Produkt mit gleichen Faktoren als Potenz scheiben und umgekehrt</v>
@@ -7171,7 +7192,7 @@
         <v>ZuVGaZ1.1.2C1_desc</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Kompetenzraster!G12</f>
         <v>Zahlen in wissenschaftlicher Schreibweise mit positiven und negativen Exponenten lesen und schreiben</v>
@@ -7181,7 +7202,7 @@
         <v>ZuVGaZ1.1.2D1_desc</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>Kompetenzraster!G13</f>
         <v>Zahlen in wissenschaftlicher Schreibweise mit positiven und negativen Exponenten addieren, subtrahieren, multiplizieren, dividieren</v>
@@ -7191,7 +7212,7 @@
         <v>ZuVGaZ1.1.2E1_desc</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>Kompetenzraster!G14</f>
         <v>Systematische Aufgabenfolgen bilden, weiterführen, verändern und beschreiben</v>
@@ -7203,8 +7224,11 @@
       <c r="C14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>Kompetenzraster!G15</f>
         <v>Gesetzmässigkeiten im Bereich der natürlichen Zahlen erforschen (z.B mithilfe der Stellentafel) und mit Beispielen konkretisieren</v>
@@ -7216,8 +7240,11 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>Kompetenzraster!G16</f>
         <v>Figurenfolgen in systematische Aufgabenfolgen übersetzen</v>
@@ -7227,7 +7254,7 @@
         <v>ZuVGaZ1.1.3B1_desc</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Kompetenzraster!G17</f>
         <v>Arithmetische Zusammenhänge durch systematisches Variieren von Zahlen, Stellenwerten und Operationen erforschen und Beobachtungen festhalten</v>
@@ -7237,7 +7264,7 @@
         <v>ZuVGaZ1.1.3C1_desc</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Kompetenzraster!G18</f>
         <v>Arithmetische Zusammenhänge erforschen, Strukturen auf andere Zahlbeispiele übertragen und Beobachtungen festhalten</v>
@@ -7247,7 +7274,7 @@
         <v>ZuVGaZ1.1.3D1_desc</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Kompetenzraster!G19</f>
         <v>Zahlen mit Komma lesen, schreiben und ordnen</v>
@@ -7259,8 +7286,11 @@
       <c r="C19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Kompetenzraster!G20</f>
         <v>In Schritten vorwärts und rückwärts zählen</v>
@@ -7272,8 +7302,11 @@
       <c r="C20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>Kompetenzraster!G21</f>
         <v>Brüche mit den Nennern 2, 3, 4, 5, 6, 8, 10, 12, 20, 50, 100 ordnen und auf dem Zahlenstarhl einzeichnen</v>
@@ -7286,7 +7319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>Kompetenzraster!G22</f>
         <v>positive und negative Zahlen auf dem Zahlenstral ordnen</v>
@@ -7299,7 +7332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>Kompetenzraster!G23</f>
         <v>Potenzen mit natürlichenm Exponenten lesen, schreiben und berechnen</v>
@@ -7309,7 +7342,7 @@
         <v>ZuVGeZ1.2.1D1_desc</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>Kompetenzraster!G24</f>
         <v>Zahlen mit Komma runden</v>
@@ -7321,8 +7354,11 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>Kompetenzraster!G25</f>
         <v>Summen und Differenzen von Zahlen mit Komma überschlagen</v>
@@ -7332,7 +7368,7 @@
         <v>ZuVGeZ1.2.2B1_desc</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>Kompetenzraster!G26</f>
         <v>Rechenergebnisse sinnvoll runden</v>
@@ -7342,7 +7378,7 @@
         <v>ZuVGeZ1.2.2C1_desc</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>Kompetenzraster!G27</f>
         <v>Produkte und Quotienten von Zahlen mit Komma überschlagen</v>
@@ -7352,7 +7388,7 @@
         <v>ZuVGeZ1.2.2D1_desc</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>Kompetenzraster!G28</f>
         <v>Zahlen bis 5 Wertziffern addieren und subtrahieren</v>
@@ -7364,8 +7400,11 @@
       <c r="C28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>Kompetenzraster!G29</f>
         <v>Zahlen bis 5 Wertziffern multiplizieren und die Ergebnisse überprüfen</v>
@@ -7375,7 +7414,7 @@
         <v>ZuVGeZ1.2.3B1_desc</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>Kompetenzraster!G30</f>
         <v>Brüche mit den Nennern 2, 3, 4, 5, 6, 8, 10, 12, 20, 50, 100  kürzen, erweitern, addieren und subtrahieren</v>
@@ -7385,7 +7424,7 @@
         <v>ZuVGeZ1.2.3B2_desc</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>Kompetenzraster!G31</f>
         <v>Brüche mit den Nennern 2, 3, 4, 5, 6, 8, 10, 12, 20, 50, 100  multiplizieren</v>
@@ -7395,7 +7434,7 @@
         <v>ZuVGeZ1.2.3C1_desc</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>Kompetenzraster!G32</f>
         <v>Grundoperationen mit rationalen Zahlen ausführen und durch Umkehroperationen überprüfen</v>
@@ -7405,7 +7444,7 @@
         <v>ZuVGeZ1.2.3D1_desc</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>Kompetenzraster!G33</f>
         <v>Brüche darstellen und vergleichen sowie Darstellungen Interpretieren</v>
@@ -7417,8 +7456,11 @@
       <c r="C33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>Kompetenzraster!G34</f>
         <v>Brüche (Nenner 2, 3, 4, 5, 6, 8, 10, 20,  50, 100, 1'000), Zahlen mit Komma und Prozentzahlen je in die beiden anderen Schreibweisen übertragen. 
@@ -7429,7 +7471,7 @@
         <v>ZuVGeZ1.2.4B1_desc</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>Kompetenzraster!G35</f>
         <v>Zahlenfolgen mit positiven rationalen Zahlen beschreiben. Eigenschaften von rationalen Zahlen erforschen und beschreiben
@@ -7440,7 +7482,7 @@
         <v>ZuVGeZ1.2.4C1_desc</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>Kompetenzraster!G36</f>
         <v>Anzahl Nachkommmastellen bei Produkten und Quotienten von Zahlen mit Komma erforschen und begründen</v>
@@ -7450,7 +7492,7 @@
         <v>ZuVGeZ1.2.4D1_desc</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>Kompetenzraster!G37</f>
         <v>Zahlen mit Klammern auswerten</v>
@@ -7462,8 +7504,11 @@
       <c r="C37" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>Kompetenzraster!G38</f>
         <v>Zahlenterme mit Klammern und Grundoperationen (Punkt vor Strich) berechnen</v>
@@ -7476,7 +7521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>Kompetenzraster!G39</f>
         <v>Terme mit Variablen addieren und subtrahieren</v>
@@ -7486,7 +7531,7 @@
         <v>ZuVAl1.3.1C1_desc</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f>Kompetenzraster!G40</f>
         <v>Terme mit Variablen umformen bzw. sinnvoll vereinfachen (z.B. Terme mit Binomen) 
@@ -7497,7 +7542,7 @@
         <v>ZuVAl1.3.1D1_desc</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>Kompetenzraster!G41</f>
         <v>Terme mit Potenzen und Quadratwurzeln umformen und berechnen</v>
@@ -7507,7 +7552,7 @@
         <v>ZuVAl1.3.1E1_desc</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f>Kompetenzraster!G42</f>
         <v>Gleichwertigkeit von zwei Zahlentermen überprüfen</v>
@@ -7519,8 +7564,11 @@
       <c r="C42" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f>Kompetenzraster!G43</f>
         <v>Gleichungen mit einer Variablen durch Einsetzen oder Umkehroperationen lösen und überprüfen</v>
@@ -7530,7 +7578,7 @@
         <v>ZuVAl1.3.2B1_desc</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f>Kompetenzraster!G44</f>
         <v>lineare Gleichungen mit einer Variablen mit Äquivalenzumformungen lösen und überprüfen</v>
@@ -7540,7 +7588,7 @@
         <v>ZuVAl1.3.2C1_desc</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f>Kompetenzraster!G45</f>
         <v>Gleichungen sprachlich deuten und zu Texten Gleichungen finden</v>
@@ -7550,7 +7598,7 @@
         <v>ZuVAl1.3.2D1_desc</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f>Kompetenzraster!G46</f>
         <v>Quadratische Gleichungen durch Faktorzerlegung lösen</v>
@@ -7560,7 +7608,7 @@
         <v>ZuVAl1.3.2E1_desc</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f>Kompetenzraster!G47</f>
         <v>Bruchgleichungen lösen</v>
@@ -7570,7 +7618,7 @@
         <v>ZuVAl1.3.2E2_desc</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>Kompetenzraster!G48</f>
         <v>Figurenfolgen und arithmetische Muster weiterführen</v>
@@ -7582,8 +7630,11 @@
       <c r="C48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f>Kompetenzraster!G49</f>
         <v>zu Figurenfolgen oder arithmetischen Mustern Gesetzmässigkeiten formulieren</v>
@@ -7593,7 +7644,7 @@
         <v>ZuVAl1.3.3B1_desc</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f>Kompetenzraster!G50</f>
         <v>Arithmetische und algebraische Terme veranschaulichen, insbesondere mit Text, Symbolen und Skizzen</v>
@@ -7603,7 +7654,7 @@
         <v>ZuVAl1.3.3C1_desc</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f>Kompetenzraster!G51</f>
         <v>Terme geometrisch interpretieren
@@ -7614,7 +7665,7 @@
         <v>ZuVAl1.3.3D1_desc</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f>Kompetenzraster!G52</f>
         <v>Zahlen und Operationen in Buchstabentermen systematisch variieren
@@ -7625,7 +7676,7 @@
         <v>ZuVAl1.3.3E1_desc</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f>Kompetenzraster!G53</f>
         <v>Skizzen und Zeichnungen nachvollziehen sowie mit Rastern, Zirkel und Geodreieck (Kreise, Parallelen, Rechtewinkel, Strecken) zeichnen</v>
@@ -7637,8 +7688,11 @@
       <c r="C53" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f>Kompetenzraster!G54</f>
         <v>Winkel übertragen, messen und konstruieren</v>
@@ -7648,7 +7702,7 @@
         <v>FuRGdE2.1.1B1_desc</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f>Kompetenzraster!G55</f>
         <v>Figuren mit dem Geodreieck konstruieren, zerlegen, zusammenfügen und deren Grösse ändern</v>
@@ -7658,7 +7712,7 @@
         <v>FuRGdE2.1.1B2_desc</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f>Kompetenzraster!G56</f>
         <v>Winkelhalbierende, Mittelsenkrechte und einfache Figuren korrekt beschriften sowie mit Geodreick und Zirkel konstruieren</v>
@@ -7668,7 +7722,7 @@
         <v>FuRGdE2.1.1C1_desc</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>Kompetenzraster!G57</f>
         <v>Figuren spiegeln (Punkspiegelung, Achsenspiegelung) und verschieben un entsprechende Abbildungen erkennen</v>
@@ -7678,7 +7732,7 @@
         <v>FuRGdE2.1.1C2_desc</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f>Kompetenzraster!G58</f>
         <v>Figuren mit Zirkel und Geodreieck drehen</v>
@@ -7688,7 +7742,7 @@
         <v>FuRGdE2.1.1D1_desc</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f>Kompetenzraster!G59</f>
         <v>Figuren bei gegebenem Streckfaktor und Streckzentrum strecken</v>
@@ -7698,7 +7752,7 @@
         <v>FuRGdE2.1.1E1_desc</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f>Kompetenzraster!G60</f>
         <v>den Umfang von Vielecken messen, auszählen und berechnen sowie den Flächeninhalt von Quadraten und Rechtecken berechnen</v>
@@ -7710,8 +7764,11 @@
       <c r="C60" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f>Kompetenzraster!G61</f>
         <v>den Flächeninhalt von nicht rechteckigen Figuren in Rastern annähernd besteimmen</v>
@@ -7721,7 +7778,7 @@
         <v>FuRGdE2.1.2B1_desc</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
         <f>Kompetenzraster!G62</f>
         <v>Winkel in Figuren durch vergleichen und berechnen bestimmen</v>
@@ -7731,7 +7788,7 @@
         <v>FuRGdE2.1.2C1_desc</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f>Kompetenzraster!G63</f>
         <v>den Flächeninhalt von Drei- und Vierecken berechnen unter anderem auch mithilfe des Satzes von Pytagoras</v>
@@ -7741,7 +7798,7 @@
         <v>FuRGdE2.1.2C2_desc</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f>Kompetenzraster!G64</f>
         <v>den Umfang und den Flächeninhalt von Kreisen berechnen</v>
@@ -7754,7 +7811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f>Kompetenzraster!G65</f>
         <v>flexibel die Formeln zur Berechnung des Flächeninhalts von Drei- und Vierecken anwenden</v>
@@ -7764,7 +7821,7 @@
         <v>FuRGdE2.1.2D2_desc</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f>Kompetenzraster!G66</f>
         <v>Strecken und Flächeninhalte von Kreissektoren und Kreisringen berechnen</v>
@@ -7774,7 +7831,7 @@
         <v>FuRGdE2.1.2E1_desc</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f>Kompetenzraster!G67</f>
         <v>Quadrate und Rechntecke systematisch variieren, Beoachtungen festhalten und Vermutungen formulieren</v>
@@ -7786,8 +7843,11 @@
       <c r="C67" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f>Kompetenzraster!G68</f>
         <v>beim Erforschen geometrischer Beziehungen Vermutungen formulieren, überprüfen und allenfalls neue Vermutungen formulieren</v>
@@ -7797,7 +7857,7 @@
         <v>FuRGdE2.1.3B1_desc</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f>Kompetenzraster!G69</f>
         <v>Figuren systematisch variieren, zerlegen und Auswirkungen erforschen</v>
@@ -7807,7 +7867,7 @@
         <v>FuRGdE2.1.3C1_desc</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
         <f>Kompetenzraster!G70</f>
         <v>Aussagen und Flächenformeln zu Drei- und Vierecken mit Skizzen und Modellen belegen</v>
@@ -7817,7 +7877,7 @@
         <v>FuRGdE2.1.3C2_desc</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
         <f>Kompetenzraster!G71</f>
         <v>geometrische Beziehungen in Vielecken- insbesondere zwischen Winkeln, Längen und Flächen - variieren und dazu Vermutungen austauschen</v>
@@ -7827,7 +7887,7 @@
         <v>FuRGdE2.1.3D1_desc</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
         <f>Kompetenzraster!G72</f>
         <v>Aussagen zu geometrischen Beziehungen im Dreieck, Viereck und Kreis überprüfen</v>
@@ -7837,7 +7897,7 @@
         <v>FuRGdE2.1.3E1_desc</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
         <f>Kompetenzraster!G73</f>
         <v>Wege und Lagebeziehungen skizzieren bzw. entsprechende Pläne nutzen</v>
@@ -7849,8 +7909,11 @@
       <c r="C73" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f>Kompetenzraster!G74</f>
         <v>zu Koordinaten Figuren zueichnen sowie die Koordinaten von Punkten bestimmen</v>
@@ -7860,7 +7923,7 @@
         <v>FuRGdE2.1.4B1_desc</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
         <f>Kompetenzraster!G75</f>
         <v>Karten lesen und Streckenlängen aufgrund von Maastabangaben bestimmen und umgekehrt</v>
@@ -7870,7 +7933,7 @@
         <v>FuRGdE2.1.4C1_desc</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
         <f>Kompetenzraster!G76</f>
         <v>Abbildungen im Koordinatensystem nach Anweisungen ausführenb und verändern</v>
@@ -7880,7 +7943,7 @@
         <v>FuRGdE2.1.4D1_desc</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
         <f>Kompetenzraster!G77</f>
         <v>einen Wohnungsplan nach Masstab zeichnen bzw. entsprechender Plänse lesen</v>
@@ -7890,7 +7953,7 @@
         <v>FuRGdE2.1.4D2_desc</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
         <f>Kompetenzraster!G78</f>
         <v>aufgrund von Plänen reale Flächeninhalte berechnen</v>
@@ -7900,7 +7963,7 @@
         <v>FuRGdE2.1.4E1_desc</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
         <f>Kompetenzraster!G79</f>
         <v>aus Quadraten und Rechtecken Würfel und Quader herstellen und Quader in Quadrate zerlegen</v>
@@ -7912,8 +7975,11 @@
       <c r="C79" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
         <f>Kompetenzraster!G80</f>
         <v>aus Quadern zusammengesetze Körper skizzieren und beschreiben
@@ -7924,7 +7990,7 @@
         <v>FuRGiR2.2.1B1_desc</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
         <f>Kompetenzraster!G81</f>
         <v>Grundriss, Schrägbild, Aufsicht, Vorderansicht und Seitenansicht von rechtwinkligen Körper in einem Raster zeichen</v>
@@ -7934,7 +8000,7 @@
         <v>FuRGiR2.2.1C1_desc</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
         <f>Kompetenzraster!G82</f>
         <v>Prismen und Pyramiden skizzieren und als Schrägbild, in der Auf- und Seitenansicht sowie als Netz darstellen</v>
@@ -7944,7 +8010,7 @@
         <v>FuRGiR2.2.1D1_desc</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
         <f>Kompetenzraster!G83</f>
         <v>Skizzen für massstabgetreue Modelle anfertigen oder Modelle herstellen</v>
@@ -7954,7 +8020,7 @@
         <v>FuRGiR2.2.1E1_desc</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
         <f>Kompetenzraster!G84</f>
         <v>Quader und Würfel in der Vorstellung kippen und drehen</v>
@@ -7966,8 +8032,11 @@
       <c r="C84" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
         <f>Kompetenzraster!G85</f>
         <v>Quader und Würfel in der Vorstellunge zerlegen und zusammenfügen</v>
@@ -7977,7 +8046,7 @@
         <v>FuRGiR2.2.2B1_desc</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
         <f>Kompetenzraster!G86</f>
         <v>Körper in der Vorstellung drehen und kippen</v>
@@ -7987,7 +8056,7 @@
         <v>FuRGiR2.2.2C1_desc</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
         <f>Kompetenzraster!G87</f>
         <v>Körper in der Vorstellung veränder und Ergebnisse beschreiben</v>
@@ -7997,7 +8066,7 @@
         <v>FuRGiR2.2.2D1_desc</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
         <f>Kompetenzraster!G88</f>
         <v>Quader aus Einheitswürfeln zusammenbauen und das Volumen auszählen</v>
@@ -8009,8 +8078,11 @@
       <c r="C88" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
         <f>Kompetenzraster!G89</f>
         <v>Volumen und Seitenflächen von Quadern berechnen</v>
@@ -8020,7 +8092,7 @@
         <v>FuRGiR2.2.3B1_desc</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
         <f>Kompetenzraster!G90</f>
         <v>das Volumen beliebiger Körper durch Vergleich mit Quadern schätzen
@@ -8031,7 +8103,7 @@
         <v>FuRGiR2.2.3C1_desc</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
         <f>Kompetenzraster!G91</f>
         <v>Kantenlängen, Flächen und Volumen an geraden Prismen und Zylindern berechnen</v>
@@ -8041,7 +8113,7 @@
         <v>FuRGiR2.2.3D1_desc</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
         <f>Kompetenzraster!G92</f>
         <v>Strecken, Flächen und Volumen an Pyramiden, Kegeln und Kugeln berechnen
@@ -8052,7 +8124,7 @@
         <v>FuRGiR2.2.3E1_desc</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
         <f>Kompetenzraster!G93</f>
         <v>sich bei Längen-, Flächen-, Gewichts- und Zeitmassen an Referenzgrössen orientieren, sowie deren Abkürzung verwenden</v>
@@ -8064,8 +8136,11 @@
       <c r="C93" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
         <f>Kompetenzraster!G94</f>
         <v>sich bei Raum- und Hohlmassen an Referenzgrössen orientieren, sowie deren Abkürzungen verwenden</v>
@@ -8078,7 +8153,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
         <f>Kompetenzraster!G95</f>
         <v>zusammengesetzte Masseinheiten und deren Abkürzungen verwenden</v>
@@ -8091,7 +8166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
         <f>Kompetenzraster!G96</f>
         <v>das System der dezimalen Masseinheiten (SI-System) und deren Vorsätze nutzen und verstehen</v>
@@ -8104,7 +8179,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
         <f>Kompetenzraster!G97</f>
         <v>Grössen (Geld, Längen, Gewicht bzw. Masse) schätzen, berstimmen, vergleichen, runden, addieren, subtrahieren und umwandeln</v>
@@ -8116,8 +8191,11 @@
       <c r="C97" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
         <f>Kompetenzraster!G98</f>
         <v>Flächeninhalte und Volumen in einer geeigneten Masseinheit schätzen und umwandeln</v>
@@ -8127,7 +8205,7 @@
         <v>GFDZGuM3.1.2B1_desc</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
         <f>Kompetenzraster!G99</f>
         <v>Sachsituationen zwischen Grössen mit Przentzahlen beschreiben</v>
@@ -8137,7 +8215,7 @@
         <v>GFDZGuM3.1.2C1_desc</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
         <f>Kompetenzraster!G100</f>
         <v>Zeiteinheiten situationsgerecht auswählen und diese umwandeln</v>
@@ -8147,7 +8225,7 @@
         <v>GFDZGuM3.1.2C2_desc</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="str">
         <f>Kompetenzraster!G101</f>
         <v>flexibel mit Raum- und Hohlmasse umgehen</v>
@@ -8157,7 +8235,7 @@
         <v>GFDZGuM3.1.2D1_desc</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
         <f>Kompetenzraster!G102</f>
         <v>Berechnungen mit zusammengesetzten Masszahlen durchführen und entsprechende Masseinheiten umrechnen</v>
@@ -8167,7 +8245,7 @@
         <v>GFDZGuM3.1.3E1_desc</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
         <f>Kompetenzraster!G103</f>
         <v>Datensätzen ordnen sowie Mittelwert, Maximum und Minimum bestimmen</v>
@@ -8179,8 +8257,11 @@
       <c r="C103" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
         <f>Kompetenzraster!G104</f>
         <v>Alltagssituationen in mathematische Sprache übersetzebn und geeignete Masseinheiten wählen</v>
@@ -8190,7 +8271,7 @@
         <v>GFDZGuM3.1.3B1_desc</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
         <f>Kompetenzraster!G105</f>
         <v>Daten zu verschiedenen Grössen mittels Experimenten, Messungen und Berechnungen sammeln, in einem Diagramm darstellen und interpretieren</v>
@@ -8200,7 +8281,7 @@
         <v>GFDZGuM3.1.3C1_desc</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
         <f>Kompetenzraster!G106</f>
         <v>Beziehungen zwischen verschiedenen Grössen datengestützt darstellen</v>
@@ -8210,7 +8291,7 @@
         <v>GFDZGuM3.1.3D1_desc</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
         <f>Kompetenzraster!G107</f>
         <v>Proportionalität in Sachsituationen erkennen und mit proportionalen Beziehungen rechnen</v>
@@ -8222,8 +8303,11 @@
       <c r="C107" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
         <f>Kompetenzraster!G108</f>
         <v>zu einer proportionalen Wertetabelle Zusammenhänge beschreiben</v>
@@ -8232,8 +8316,11 @@
         <f>Kompetenzraster!H108</f>
         <v>GFDZFZP3.2.1B1_desc</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
         <f>Kompetenzraster!G109</f>
         <v>Prozentangaben als proportionale Zuordnungen verstehen und Prozentrechnungen ausführen</v>
@@ -8242,8 +8329,11 @@
         <f>Kompetenzraster!H109</f>
         <v>GFDZFZP3.2.1C1_desc</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
         <f>Kompetenzraster!G110</f>
         <v>umgekehrt bzw. indirekt proportionalen Beziehungen erkennen und damit rechnen</v>
@@ -8253,7 +8343,7 @@
         <v>GFDZFZP3.2.1D1_desc</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
         <f>Kompetenzraster!G111</f>
         <v>verschiedene funktionale Zusammenhänge in Sachsituationen erkennen</v>
@@ -8263,7 +8353,7 @@
         <v>GFDZFZP3.2.1F1_desc</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
         <f>Kompetenzraster!G112</f>
         <v>funktionale Zusammenhänge in Wertetabellen erfassen</v>
@@ -8273,6 +8363,9 @@
         <v>GFDZFZP3.2.2A1_desc</v>
       </c>
       <c r="C112" t="s">
+        <v>23</v>
+      </c>
+      <c r="D112" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minimal explorer functionality working
</commit_message>
<xml_diff>
--- a/Berufsprofile-Kompetenzraster.xlsx
+++ b/Berufsprofile-Kompetenzraster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielschmocker/Documents/Projekte/Benjamin/Berufsprofile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15843DC9-002B-DD4D-B4B2-146F1B0ABA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD303796-DEFE-184D-ABB7-2A6E328A9469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompetenzraster" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="212">
   <si>
     <t>lable</t>
   </si>
@@ -661,6 +661,27 @@
   </si>
   <si>
     <t>detailhandelsass</t>
+  </si>
+  <si>
+    <t>AgrarpraktikerIn EBA</t>
+  </si>
+  <si>
+    <t>agrarpra</t>
+  </si>
+  <si>
+    <t>DetailhandelsfachFrauMann EFZ</t>
+  </si>
+  <si>
+    <t>detailhandelsfach</t>
+  </si>
+  <si>
+    <t>alle As</t>
+  </si>
+  <si>
+    <t>InformatikerIn EFZ</t>
+  </si>
+  <si>
+    <t>informatik</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7055,21 +7076,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8200FB-305B-E64F-B9C4-B1DA92FAD6FD}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.33203125" customWidth="1"/>
+    <col min="1" max="1" width="81.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7082,8 +7104,20 @@
       <c r="D1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>202</v>
       </c>
@@ -7093,8 +7127,17 @@
       <c r="D2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>Kompetenzraster!G2</f>
         <v>Grundoperationen mit natürlichen Zahlen durchführen</v>
@@ -7109,8 +7152,20 @@
       <c r="D3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Kompetenzraster!G3</f>
         <v>Zahlen erkennen, die durch 2, 5, 10, 100, 1'000 teibar sind</v>
@@ -7125,8 +7180,20 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Kompetenzraster!G4</f>
         <v>Zahlen bis 1 Milliarde lesen udn schreiben</v>
@@ -7141,8 +7208,17 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Kompetenzraster!G5</f>
         <v>Grundoperationen mit natürlichen Zahlen überschlagen</v>
@@ -7154,8 +7230,17 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>Kompetenzraster!G6</f>
         <v>Teilbarkeitsregeln (3,4,6,8,9,25,50) nutzen und Teiler natürlicher Zahlen bestimmen</v>
@@ -7164,8 +7249,11 @@
         <f>Kompetenzraster!H6</f>
         <v>ZuVGaZ1.1.1C1_desc</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Kompetenzraster!G7</f>
         <v>Grundoperationnen mit ganzen Zahlen durchführen</v>
@@ -7174,8 +7262,11 @@
         <f>Kompetenzraster!H7</f>
         <v>ZuVGaZ1.1.1D1_desc</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>Kompetenzraster!G8</f>
         <v>natürliche Zahlen in Primfaktoren zerlegen</v>
@@ -7184,8 +7275,11 @@
         <f>Kompetenzraster!H8</f>
         <v>ZuVGaZ1.1.1E1_desc</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Kompetenzraster!G9</f>
         <v>Die ersten 20 Quadratzahlen ohne TR bestimmen und geometrisch deuten</v>
@@ -7200,8 +7294,20 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Kompetenzraster!G10</f>
         <v>Wurzeln und Potenzen mit dem Rechner berechnen, sowie einfache Wurzeln unt Potenzen im Kopf bestimmen</v>
@@ -7210,8 +7316,14 @@
         <f>Kompetenzraster!H10</f>
         <v>ZuVGaZ1.1.2B1_desc</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Kompetenzraster!G11</f>
         <v>Ein Produkt mit gleichen Faktoren als Potenz scheiben und umgekehrt</v>
@@ -7220,8 +7332,11 @@
         <f>Kompetenzraster!H11</f>
         <v>ZuVGaZ1.1.2C1_desc</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>Kompetenzraster!G12</f>
         <v>Zahlen in wissenschaftlicher Schreibweise mit positiven und negativen Exponenten lesen und schreiben</v>
@@ -7230,8 +7345,11 @@
         <f>Kompetenzraster!H12</f>
         <v>ZuVGaZ1.1.2D1_desc</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>Kompetenzraster!G13</f>
         <v>Zahlen in wissenschaftlicher Schreibweise mit positiven und negativen Exponenten addieren, subtrahieren, multiplizieren, dividieren</v>
@@ -7240,8 +7358,11 @@
         <f>Kompetenzraster!H13</f>
         <v>ZuVGaZ1.1.2E1_desc</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>Kompetenzraster!G14</f>
         <v>Systematische Aufgabenfolgen bilden, weiterführen, verändern und beschreiben</v>
@@ -7256,8 +7377,20 @@
       <c r="D15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>Kompetenzraster!G15</f>
         <v>Gesetzmässigkeiten im Bereich der natürlichen Zahlen erforschen (z.B mithilfe der Stellentafel) und mit Beispielen konkretisieren</v>
@@ -7272,8 +7405,20 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Kompetenzraster!G16</f>
         <v>Figurenfolgen in systematische Aufgabenfolgen übersetzen</v>
@@ -7282,8 +7427,14 @@
         <f>Kompetenzraster!H16</f>
         <v>ZuVGaZ1.1.3B1_desc</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Kompetenzraster!G17</f>
         <v>Arithmetische Zusammenhänge durch systematisches Variieren von Zahlen, Stellenwerten und Operationen erforschen und Beobachtungen festhalten</v>
@@ -7292,8 +7443,11 @@
         <f>Kompetenzraster!H17</f>
         <v>ZuVGaZ1.1.3C1_desc</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Kompetenzraster!G18</f>
         <v>Arithmetische Zusammenhänge erforschen, Strukturen auf andere Zahlbeispiele übertragen und Beobachtungen festhalten</v>
@@ -7302,8 +7456,11 @@
         <f>Kompetenzraster!H18</f>
         <v>ZuVGaZ1.1.3D1_desc</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Kompetenzraster!G19</f>
         <v>Zahlen mit Komma lesen, schreiben und ordnen</v>
@@ -7318,8 +7475,20 @@
       <c r="D20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>Kompetenzraster!G20</f>
         <v>In Schritten vorwärts und rückwärts zählen</v>
@@ -7334,8 +7503,17 @@
       <c r="D21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>Kompetenzraster!G21</f>
         <v>Brüche mit den Nennern 2, 3, 4, 5, 6, 8, 10, 12, 20, 50, 100 ordnen und auf dem Zahlenstarhl einzeichnen</v>
@@ -7347,8 +7525,14 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>Kompetenzraster!G22</f>
         <v>positive und negative Zahlen auf dem Zahlenstral ordnen</v>
@@ -7360,8 +7544,14 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>Kompetenzraster!G23</f>
         <v>Potenzen mit natürlichenm Exponenten lesen, schreiben und berechnen</v>
@@ -7370,8 +7560,11 @@
         <f>Kompetenzraster!H23</f>
         <v>ZuVGeZ1.2.1D1_desc</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>Kompetenzraster!G24</f>
         <v>Zahlen mit Komma runden</v>
@@ -7386,8 +7579,20 @@
       <c r="D25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>Kompetenzraster!G25</f>
         <v>Summen und Differenzen von Zahlen mit Komma überschlagen</v>
@@ -7396,8 +7601,17 @@
         <f>Kompetenzraster!H25</f>
         <v>ZuVGeZ1.2.2B1_desc</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>Kompetenzraster!G26</f>
         <v>Rechenergebnisse sinnvoll runden</v>
@@ -7406,8 +7620,14 @@
         <f>Kompetenzraster!H26</f>
         <v>ZuVGeZ1.2.2C1_desc</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>Kompetenzraster!G27</f>
         <v>Produkte und Quotienten von Zahlen mit Komma überschlagen</v>
@@ -7416,8 +7636,11 @@
         <f>Kompetenzraster!H27</f>
         <v>ZuVGeZ1.2.2D1_desc</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>Kompetenzraster!G28</f>
         <v>Zahlen bis 5 Wertziffern addieren und subtrahieren</v>
@@ -7432,8 +7655,20 @@
       <c r="D29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>Kompetenzraster!G29</f>
         <v>Zahlen bis 5 Wertziffern multiplizieren und die Ergebnisse überprüfen</v>
@@ -7442,8 +7677,11 @@
         <f>Kompetenzraster!H29</f>
         <v>ZuVGeZ1.2.3B1_desc</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>Kompetenzraster!G30</f>
         <v>Brüche mit den Nennern 2, 3, 4, 5, 6, 8, 10, 12, 20, 50, 100  kürzen, erweitern, addieren und subtrahieren</v>
@@ -7452,8 +7690,11 @@
         <f>Kompetenzraster!H30</f>
         <v>ZuVGeZ1.2.3B2_desc</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>Kompetenzraster!G31</f>
         <v>Brüche mit den Nennern 2, 3, 4, 5, 6, 8, 10, 12, 20, 50, 100  multiplizieren</v>
@@ -7462,8 +7703,11 @@
         <f>Kompetenzraster!H31</f>
         <v>ZuVGeZ1.2.3C1_desc</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>Kompetenzraster!G32</f>
         <v>Grundoperationen mit rationalen Zahlen ausführen und durch Umkehroperationen überprüfen</v>
@@ -7472,8 +7716,11 @@
         <f>Kompetenzraster!H32</f>
         <v>ZuVGeZ1.2.3D1_desc</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>Kompetenzraster!G33</f>
         <v>Brüche darstellen und vergleichen sowie Darstellungen Interpretieren</v>
@@ -7488,8 +7735,20 @@
       <c r="D34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>Kompetenzraster!G34</f>
         <v>Brüche (Nenner 2, 3, 4, 5, 6, 8, 10, 20,  50, 100, 1'000), Zahlen mit Komma und Prozentzahlen je in die beiden anderen Schreibweisen übertragen. 
@@ -7499,8 +7758,14 @@
         <f>Kompetenzraster!H34</f>
         <v>ZuVGeZ1.2.4B1_desc</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>Kompetenzraster!G35</f>
         <v>Zahlenfolgen mit positiven rationalen Zahlen beschreiben. Eigenschaften von rationalen Zahlen erforschen und beschreiben
@@ -7510,8 +7775,11 @@
         <f>Kompetenzraster!H35</f>
         <v>ZuVGeZ1.2.4C1_desc</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>Kompetenzraster!G36</f>
         <v>Anzahl Nachkommmastellen bei Produkten und Quotienten von Zahlen mit Komma erforschen und begründen</v>
@@ -7520,8 +7788,11 @@
         <f>Kompetenzraster!H36</f>
         <v>ZuVGeZ1.2.4D1_desc</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>Kompetenzraster!G37</f>
         <v>Zahlen mit Klammern auswerten</v>
@@ -7536,8 +7807,20 @@
       <c r="D38" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>Kompetenzraster!G38</f>
         <v>Zahlenterme mit Klammern und Grundoperationen (Punkt vor Strich) berechnen</v>
@@ -7549,8 +7832,14 @@
       <c r="C39" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f>Kompetenzraster!G39</f>
         <v>Terme mit Variablen addieren und subtrahieren</v>
@@ -7559,8 +7848,11 @@
         <f>Kompetenzraster!H39</f>
         <v>ZuVAl1.3.1C1_desc</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>Kompetenzraster!G40</f>
         <v>Terme mit Variablen umformen bzw. sinnvoll vereinfachen (z.B. Terme mit Binomen) 
@@ -7570,8 +7862,11 @@
         <f>Kompetenzraster!H40</f>
         <v>ZuVAl1.3.1D1_desc</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f>Kompetenzraster!G41</f>
         <v>Terme mit Potenzen und Quadratwurzeln umformen und berechnen</v>
@@ -7580,8 +7875,11 @@
         <f>Kompetenzraster!H41</f>
         <v>ZuVAl1.3.1E1_desc</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f>Kompetenzraster!G42</f>
         <v>Gleichwertigkeit von zwei Zahlentermen überprüfen</v>
@@ -7596,8 +7894,20 @@
       <c r="D43" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f>Kompetenzraster!G43</f>
         <v>Gleichungen mit einer Variablen durch Einsetzen oder Umkehroperationen lösen und überprüfen</v>
@@ -7606,8 +7916,11 @@
         <f>Kompetenzraster!H43</f>
         <v>ZuVAl1.3.2B1_desc</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f>Kompetenzraster!G44</f>
         <v>lineare Gleichungen mit einer Variablen mit Äquivalenzumformungen lösen und überprüfen</v>
@@ -7616,8 +7929,11 @@
         <f>Kompetenzraster!H44</f>
         <v>ZuVAl1.3.2C1_desc</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f>Kompetenzraster!G45</f>
         <v>Gleichungen sprachlich deuten und zu Texten Gleichungen finden</v>
@@ -7626,8 +7942,11 @@
         <f>Kompetenzraster!H45</f>
         <v>ZuVAl1.3.2D1_desc</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f>Kompetenzraster!G46</f>
         <v>Quadratische Gleichungen durch Faktorzerlegung lösen</v>
@@ -7636,8 +7955,11 @@
         <f>Kompetenzraster!H46</f>
         <v>ZuVAl1.3.2E1_desc</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>Kompetenzraster!G47</f>
         <v>Bruchgleichungen lösen</v>
@@ -7646,8 +7968,11 @@
         <f>Kompetenzraster!H47</f>
         <v>ZuVAl1.3.2E2_desc</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f>Kompetenzraster!G48</f>
         <v>Figurenfolgen und arithmetische Muster weiterführen</v>
@@ -7662,8 +7987,20 @@
       <c r="D49" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f>Kompetenzraster!G49</f>
         <v>zu Figurenfolgen oder arithmetischen Mustern Gesetzmässigkeiten formulieren</v>
@@ -7673,7 +8010,7 @@
         <v>ZuVAl1.3.3B1_desc</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f>Kompetenzraster!G50</f>
         <v>Arithmetische und algebraische Terme veranschaulichen, insbesondere mit Text, Symbolen und Skizzen</v>
@@ -7683,7 +8020,7 @@
         <v>ZuVAl1.3.3C1_desc</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f>Kompetenzraster!G51</f>
         <v>Terme geometrisch interpretieren
@@ -7693,8 +8030,11 @@
         <f>Kompetenzraster!H51</f>
         <v>ZuVAl1.3.3D1_desc</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f>Kompetenzraster!G52</f>
         <v>Zahlen und Operationen in Buchstabentermen systematisch variieren
@@ -7704,8 +8044,11 @@
         <f>Kompetenzraster!H52</f>
         <v>ZuVAl1.3.3E1_desc</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f>Kompetenzraster!G53</f>
         <v>Skizzen und Zeichnungen nachvollziehen sowie mit Rastern, Zirkel und Geodreieck (Kreise, Parallelen, Rechtewinkel, Strecken) zeichnen</v>
@@ -7720,8 +8063,20 @@
       <c r="D54" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f>Kompetenzraster!G54</f>
         <v>Winkel übertragen, messen und konstruieren</v>
@@ -7730,8 +8085,11 @@
         <f>Kompetenzraster!H54</f>
         <v>FuRGdE2.1.1B1_desc</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f>Kompetenzraster!G55</f>
         <v>Figuren mit dem Geodreieck konstruieren, zerlegen, zusammenfügen und deren Grösse ändern</v>
@@ -7740,8 +8098,11 @@
         <f>Kompetenzraster!H55</f>
         <v>FuRGdE2.1.1B2_desc</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>Kompetenzraster!G56</f>
         <v>Winkelhalbierende, Mittelsenkrechte und einfache Figuren korrekt beschriften sowie mit Geodreick und Zirkel konstruieren</v>
@@ -7750,8 +8111,11 @@
         <f>Kompetenzraster!H56</f>
         <v>FuRGdE2.1.1C1_desc</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f>Kompetenzraster!G57</f>
         <v>Figuren spiegeln (Punkspiegelung, Achsenspiegelung) und verschieben un entsprechende Abbildungen erkennen</v>
@@ -7760,8 +8124,11 @@
         <f>Kompetenzraster!H57</f>
         <v>FuRGdE2.1.1C2_desc</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f>Kompetenzraster!G58</f>
         <v>Figuren mit Zirkel und Geodreieck drehen</v>
@@ -7770,8 +8137,11 @@
         <f>Kompetenzraster!H58</f>
         <v>FuRGdE2.1.1D1_desc</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f>Kompetenzraster!G59</f>
         <v>Figuren bei gegebenem Streckfaktor und Streckzentrum strecken</v>
@@ -7781,7 +8151,7 @@
         <v>FuRGdE2.1.1E1_desc</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f>Kompetenzraster!G60</f>
         <v>den Umfang von Vielecken messen, auszählen und berechnen sowie den Flächeninhalt von Quadraten und Rechtecken berechnen</v>
@@ -7796,8 +8166,20 @@
       <c r="D61" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>23</v>
+      </c>
+      <c r="H61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
         <f>Kompetenzraster!G61</f>
         <v>den Flächeninhalt von nicht rechteckigen Figuren in Rastern annähernd besteimmen</v>
@@ -7806,8 +8188,11 @@
         <f>Kompetenzraster!H61</f>
         <v>FuRGdE2.1.2B1_desc</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f>Kompetenzraster!G62</f>
         <v>Winkel in Figuren durch vergleichen und berechnen bestimmen</v>
@@ -7817,7 +8202,7 @@
         <v>FuRGdE2.1.2C1_desc</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f>Kompetenzraster!G63</f>
         <v>den Flächeninhalt von Drei- und Vierecken berechnen unter anderem auch mithilfe des Satzes von Pytagoras</v>
@@ -7826,8 +8211,11 @@
         <f>Kompetenzraster!H63</f>
         <v>FuRGdE2.1.2C2_desc</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f>Kompetenzraster!G64</f>
         <v>den Umfang und den Flächeninhalt von Kreisen berechnen</v>
@@ -7839,8 +8227,11 @@
       <c r="C65" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f>Kompetenzraster!G65</f>
         <v>flexibel die Formeln zur Berechnung des Flächeninhalts von Drei- und Vierecken anwenden</v>
@@ -7849,8 +8240,11 @@
         <f>Kompetenzraster!H65</f>
         <v>FuRGdE2.1.2D2_desc</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f>Kompetenzraster!G66</f>
         <v>Strecken und Flächeninhalte von Kreissektoren und Kreisringen berechnen</v>
@@ -7859,8 +8253,11 @@
         <f>Kompetenzraster!H66</f>
         <v>FuRGdE2.1.2E1_desc</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f>Kompetenzraster!G67</f>
         <v>Quadrate und Rechntecke systematisch variieren, Beoachtungen festhalten und Vermutungen formulieren</v>
@@ -7875,8 +8272,20 @@
       <c r="D68" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>23</v>
+      </c>
+      <c r="F68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f>Kompetenzraster!G68</f>
         <v>beim Erforschen geometrischer Beziehungen Vermutungen formulieren, überprüfen und allenfalls neue Vermutungen formulieren</v>
@@ -7886,7 +8295,7 @@
         <v>FuRGdE2.1.3B1_desc</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
         <f>Kompetenzraster!G69</f>
         <v>Figuren systematisch variieren, zerlegen und Auswirkungen erforschen</v>
@@ -7896,7 +8305,7 @@
         <v>FuRGdE2.1.3C1_desc</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
         <f>Kompetenzraster!G70</f>
         <v>Aussagen und Flächenformeln zu Drei- und Vierecken mit Skizzen und Modellen belegen</v>
@@ -7906,7 +8315,7 @@
         <v>FuRGdE2.1.3C2_desc</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
         <f>Kompetenzraster!G71</f>
         <v>geometrische Beziehungen in Vielecken- insbesondere zwischen Winkeln, Längen und Flächen - variieren und dazu Vermutungen austauschen</v>
@@ -7916,7 +8325,7 @@
         <v>FuRGdE2.1.3D1_desc</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
         <f>Kompetenzraster!G72</f>
         <v>Aussagen zu geometrischen Beziehungen im Dreieck, Viereck und Kreis überprüfen</v>
@@ -7926,7 +8335,7 @@
         <v>FuRGdE2.1.3E1_desc</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f>Kompetenzraster!G73</f>
         <v>Wege und Lagebeziehungen skizzieren bzw. entsprechende Pläne nutzen</v>
@@ -7941,8 +8350,20 @@
       <c r="D74" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" t="s">
+        <v>23</v>
+      </c>
+      <c r="G74" t="s">
+        <v>23</v>
+      </c>
+      <c r="H74" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
         <f>Kompetenzraster!G74</f>
         <v>zu Koordinaten Figuren zueichnen sowie die Koordinaten von Punkten bestimmen</v>
@@ -7951,8 +8372,11 @@
         <f>Kompetenzraster!H74</f>
         <v>FuRGdE2.1.4B1_desc</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G75" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
         <f>Kompetenzraster!G75</f>
         <v>Karten lesen und Streckenlängen aufgrund von Maastabangaben bestimmen und umgekehrt</v>
@@ -7962,7 +8386,7 @@
         <v>FuRGdE2.1.4C1_desc</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
         <f>Kompetenzraster!G76</f>
         <v>Abbildungen im Koordinatensystem nach Anweisungen ausführenb und verändern</v>
@@ -7971,8 +8395,11 @@
         <f>Kompetenzraster!H76</f>
         <v>FuRGdE2.1.4D1_desc</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
         <f>Kompetenzraster!G77</f>
         <v>einen Wohnungsplan nach Masstab zeichnen bzw. entsprechender Plänse lesen</v>
@@ -7982,7 +8409,7 @@
         <v>FuRGdE2.1.4D2_desc</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
         <f>Kompetenzraster!G78</f>
         <v>aufgrund von Plänen reale Flächeninhalte berechnen</v>
@@ -7992,7 +8419,7 @@
         <v>FuRGdE2.1.4E1_desc</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
         <f>Kompetenzraster!G79</f>
         <v>aus Quadraten und Rechtecken Würfel und Quader herstellen und Quader in Quadrate zerlegen</v>
@@ -8007,8 +8434,20 @@
       <c r="D80" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>23</v>
+      </c>
+      <c r="F80" t="s">
+        <v>23</v>
+      </c>
+      <c r="G80" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
         <f>Kompetenzraster!G80</f>
         <v>aus Quadern zusammengesetze Körper skizzieren und beschreiben
@@ -8019,7 +8458,7 @@
         <v>FuRGiR2.2.1B1_desc</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
         <f>Kompetenzraster!G81</f>
         <v>Grundriss, Schrägbild, Aufsicht, Vorderansicht und Seitenansicht von rechtwinkligen Körper in einem Raster zeichen</v>
@@ -8029,7 +8468,7 @@
         <v>FuRGiR2.2.1C1_desc</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
         <f>Kompetenzraster!G82</f>
         <v>Prismen und Pyramiden skizzieren und als Schrägbild, in der Auf- und Seitenansicht sowie als Netz darstellen</v>
@@ -8039,7 +8478,7 @@
         <v>FuRGiR2.2.1D1_desc</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
         <f>Kompetenzraster!G83</f>
         <v>Skizzen für massstabgetreue Modelle anfertigen oder Modelle herstellen</v>
@@ -8049,7 +8488,7 @@
         <v>FuRGiR2.2.1E1_desc</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
         <f>Kompetenzraster!G84</f>
         <v>Quader und Würfel in der Vorstellung kippen und drehen</v>
@@ -8064,8 +8503,20 @@
       <c r="D85" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85" t="s">
+        <v>23</v>
+      </c>
+      <c r="G85" t="s">
+        <v>23</v>
+      </c>
+      <c r="H85" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
         <f>Kompetenzraster!G85</f>
         <v>Quader und Würfel in der Vorstellunge zerlegen und zusammenfügen</v>
@@ -8075,7 +8526,7 @@
         <v>FuRGiR2.2.2B1_desc</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
         <f>Kompetenzraster!G86</f>
         <v>Körper in der Vorstellung drehen und kippen</v>
@@ -8085,7 +8536,7 @@
         <v>FuRGiR2.2.2C1_desc</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
         <f>Kompetenzraster!G87</f>
         <v>Körper in der Vorstellung veränder und Ergebnisse beschreiben</v>
@@ -8095,7 +8546,7 @@
         <v>FuRGiR2.2.2D1_desc</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
         <f>Kompetenzraster!G88</f>
         <v>Quader aus Einheitswürfeln zusammenbauen und das Volumen auszählen</v>
@@ -8110,8 +8561,20 @@
       <c r="D89" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" t="s">
+        <v>23</v>
+      </c>
+      <c r="H89" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
         <f>Kompetenzraster!G89</f>
         <v>Volumen und Seitenflächen von Quadern berechnen</v>
@@ -8121,7 +8584,7 @@
         <v>FuRGiR2.2.3B1_desc</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
         <f>Kompetenzraster!G90</f>
         <v>das Volumen beliebiger Körper durch Vergleich mit Quadern schätzen
@@ -8132,7 +8595,7 @@
         <v>FuRGiR2.2.3C1_desc</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
         <f>Kompetenzraster!G91</f>
         <v>Kantenlängen, Flächen und Volumen an geraden Prismen und Zylindern berechnen</v>
@@ -8142,7 +8605,7 @@
         <v>FuRGiR2.2.3D1_desc</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
         <f>Kompetenzraster!G92</f>
         <v>Strecken, Flächen und Volumen an Pyramiden, Kegeln und Kugeln berechnen
@@ -8153,7 +8616,7 @@
         <v>FuRGiR2.2.3E1_desc</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
         <f>Kompetenzraster!G93</f>
         <v>sich bei Längen-, Flächen-, Gewichts- und Zeitmassen an Referenzgrössen orientieren, sowie deren Abkürzung verwenden</v>
@@ -8168,8 +8631,20 @@
       <c r="D94" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" t="s">
+        <v>23</v>
+      </c>
+      <c r="F94" t="s">
+        <v>23</v>
+      </c>
+      <c r="G94" t="s">
+        <v>23</v>
+      </c>
+      <c r="H94" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
         <f>Kompetenzraster!G94</f>
         <v>sich bei Raum- und Hohlmassen an Referenzgrössen orientieren, sowie deren Abkürzungen verwenden</v>
@@ -8181,8 +8656,14 @@
       <c r="C95" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" t="s">
+        <v>23</v>
+      </c>
+      <c r="G95" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
         <f>Kompetenzraster!G95</f>
         <v>zusammengesetzte Masseinheiten und deren Abkürzungen verwenden</v>
@@ -8194,8 +8675,11 @@
       <c r="C96" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
         <f>Kompetenzraster!G96</f>
         <v>das System der dezimalen Masseinheiten (SI-System) und deren Vorsätze nutzen und verstehen</v>
@@ -8207,8 +8691,11 @@
       <c r="C97" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
         <f>Kompetenzraster!G97</f>
         <v>Grössen (Geld, Längen, Gewicht bzw. Masse) schätzen, berstimmen, vergleichen, runden, addieren, subtrahieren und umwandeln</v>
@@ -8223,8 +8710,20 @@
       <c r="D98" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" t="s">
+        <v>23</v>
+      </c>
+      <c r="G98" t="s">
+        <v>23</v>
+      </c>
+      <c r="H98" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
         <f>Kompetenzraster!G98</f>
         <v>Flächeninhalte und Volumen in einer geeigneten Masseinheit schätzen und umwandeln</v>
@@ -8233,8 +8732,17 @@
         <f>Kompetenzraster!H98</f>
         <v>GFDZGuM3.1.2B1_desc</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" t="s">
+        <v>23</v>
+      </c>
+      <c r="F99" t="s">
+        <v>23</v>
+      </c>
+      <c r="G99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
         <f>Kompetenzraster!G99</f>
         <v>Sachsituationen zwischen Grössen mit Przentzahlen beschreiben</v>
@@ -8243,8 +8751,11 @@
         <f>Kompetenzraster!H99</f>
         <v>GFDZGuM3.1.2C1_desc</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="str">
         <f>Kompetenzraster!G100</f>
         <v>Zeiteinheiten situationsgerecht auswählen und diese umwandeln</v>
@@ -8253,8 +8764,11 @@
         <f>Kompetenzraster!H100</f>
         <v>GFDZGuM3.1.2C2_desc</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
         <f>Kompetenzraster!G101</f>
         <v>flexibel mit Raum- und Hohlmasse umgehen</v>
@@ -8263,8 +8777,11 @@
         <f>Kompetenzraster!H101</f>
         <v>GFDZGuM3.1.2D1_desc</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
         <f>Kompetenzraster!G102</f>
         <v>Berechnungen mit zusammengesetzten Masszahlen durchführen und entsprechende Masseinheiten umrechnen</v>
@@ -8273,8 +8790,11 @@
         <f>Kompetenzraster!H102</f>
         <v>GFDZGuM3.1.3E1_desc</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
         <f>Kompetenzraster!G103</f>
         <v>Datensätzen ordnen sowie Mittelwert, Maximum und Minimum bestimmen</v>
@@ -8289,8 +8809,20 @@
       <c r="D104" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" t="s">
+        <v>23</v>
+      </c>
+      <c r="F104" t="s">
+        <v>23</v>
+      </c>
+      <c r="G104" t="s">
+        <v>23</v>
+      </c>
+      <c r="H104" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
         <f>Kompetenzraster!G104</f>
         <v>Alltagssituationen in mathematische Sprache übersetzebn und geeignete Masseinheiten wählen</v>
@@ -8299,8 +8831,11 @@
         <f>Kompetenzraster!H104</f>
         <v>GFDZGuM3.1.3B1_desc</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
         <f>Kompetenzraster!G105</f>
         <v>Daten zu verschiedenen Grössen mittels Experimenten, Messungen und Berechnungen sammeln, in einem Diagramm darstellen und interpretieren</v>
@@ -8309,8 +8844,11 @@
         <f>Kompetenzraster!H105</f>
         <v>GFDZGuM3.1.3C1_desc</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
         <f>Kompetenzraster!G106</f>
         <v>Beziehungen zwischen verschiedenen Grössen datengestützt darstellen</v>
@@ -8319,8 +8857,11 @@
         <f>Kompetenzraster!H106</f>
         <v>GFDZGuM3.1.3D1_desc</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
         <f>Kompetenzraster!G107</f>
         <v>Proportionalität in Sachsituationen erkennen und mit proportionalen Beziehungen rechnen</v>
@@ -8335,8 +8876,20 @@
       <c r="D108" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" t="s">
+        <v>23</v>
+      </c>
+      <c r="F108" t="s">
+        <v>23</v>
+      </c>
+      <c r="G108" t="s">
+        <v>23</v>
+      </c>
+      <c r="H108" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
         <f>Kompetenzraster!G108</f>
         <v>zu einer proportionalen Wertetabelle Zusammenhänge beschreiben</v>
@@ -8348,8 +8901,17 @@
       <c r="D109" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" t="s">
+        <v>23</v>
+      </c>
+      <c r="F109" t="s">
+        <v>23</v>
+      </c>
+      <c r="G109" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
         <f>Kompetenzraster!G109</f>
         <v>Prozentangaben als proportionale Zuordnungen verstehen und Prozentrechnungen ausführen</v>
@@ -8361,8 +8923,17 @@
       <c r="D110" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" t="s">
+        <v>23</v>
+      </c>
+      <c r="F110" t="s">
+        <v>23</v>
+      </c>
+      <c r="G110" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
         <f>Kompetenzraster!G110</f>
         <v>umgekehrt bzw. indirekt proportionalen Beziehungen erkennen und damit rechnen</v>
@@ -8371,8 +8942,11 @@
         <f>Kompetenzraster!H110</f>
         <v>GFDZFZP3.2.1D1_desc</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
         <f>Kompetenzraster!G111</f>
         <v>verschiedene funktionale Zusammenhänge in Sachsituationen erkennen</v>
@@ -8381,8 +8955,11 @@
         <f>Kompetenzraster!H111</f>
         <v>GFDZFZP3.2.1E1_desc</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="str">
         <f>Kompetenzraster!G112</f>
         <v>funktionale Zusammenhänge in Wertetabellen erfassen</v>
@@ -8397,8 +8974,20 @@
       <c r="D113" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113" t="s">
+        <v>23</v>
+      </c>
+      <c r="F113" t="s">
+        <v>23</v>
+      </c>
+      <c r="G113" t="s">
+        <v>23</v>
+      </c>
+      <c r="H113" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="str">
         <f>Kompetenzraster!G113</f>
         <v>den Zusammenhang zwischen Werten in einer Tabelle in einem funktionalen Zusammenhang beschreiben</v>
@@ -8407,8 +8996,17 @@
         <f>Kompetenzraster!H113</f>
         <v>GFDZFZP3.2.2B2_desc</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114" t="s">
+        <v>23</v>
+      </c>
+      <c r="F114" t="s">
+        <v>23</v>
+      </c>
+      <c r="G114" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="str">
         <f>Kompetenzraster!G114</f>
         <v>Wertepaare aufgrund von Funktionsgraphen bestimmen</v>
@@ -8417,8 +9015,11 @@
         <f>Kompetenzraster!H114</f>
         <v>GFDZFZP3.2.2C1_desc</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="str">
         <f>Kompetenzraster!G115</f>
         <v>die Abhängigkeit zwier Werte mit einem Funktionsgraphen darstellen sowie Graphenverläufe interpretieren</v>
@@ -8427,8 +9028,11 @@
         <f>Kompetenzraster!H115</f>
         <v>GFDZFZP3.2.2C2_desc</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
         <f>Kompetenzraster!G116</f>
         <v>Funktionale Zusammenhänge mit Sachsituationen, Wertetabellen, Graphen und Gleichungen beschreiben</v>
@@ -8437,8 +9041,11 @@
         <f>Kompetenzraster!H116</f>
         <v>GFDZFZP3.2.2D1_desc</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G117" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="str">
         <f>Kompetenzraster!G117</f>
         <v>Funktionen im Koordinatensystem mit geeigneter Skalierung darstellen</v>
@@ -8447,8 +9054,11 @@
         <f>Kompetenzraster!H117</f>
         <v>GFDZFZP3.2.2D2_desc</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G118" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="str">
         <f>Kompetenzraster!G118</f>
         <v>den Schnittpunkt zweier Geraden algebraisch und graphisch bestimmen
@@ -8458,8 +9068,11 @@
         <f>Kompetenzraster!H118</f>
         <v>GFDZFZP3.2.2E1_desc</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G119" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="str">
         <f>Kompetenzraster!G119</f>
         <v>Behiehungen zwischen Werten erforschen und funktionale Zusammenhänge überprüfen</v>
@@ -8468,8 +9081,11 @@
         <f>Kompetenzraster!H119</f>
         <v>GFDZFZP3.2.3B1_desc</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G120" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="str">
         <f>Kompetenzraster!G120</f>
         <v>funktionale Zusammenhänge, insbesondere zu Preis-Leistung und Weg-Zeit, darstellen und begründen</v>
@@ -8478,8 +9094,11 @@
         <f>Kompetenzraster!H120</f>
         <v>GFDZFZP3.2.3C1_desc</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G121" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="str">
         <f>Kompetenzraster!G121</f>
         <v>Ergebnisse und Aussagen zu funktionalen Zusammenhängen überprüfen, insbesondere, durch Interpretation von Tabellen, Graphen und Diagrammen</v>
@@ -8488,8 +9107,11 @@
         <f>Kompetenzraster!H121</f>
         <v>GFDZFZP3.2.3D1_desc</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="str">
         <f>Kompetenzraster!G122</f>
         <v>funktionale und statistische Zusammenhänge erforschen, dazu Fragen stellen sowie Ergebnisse vergleichen</v>
@@ -8497,6 +9119,14 @@
       <c r="B123" t="str">
         <f>Kompetenzraster!H122</f>
         <v>GFDZFZP3.2.3E1_desc</v>
+      </c>
+      <c r="G123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G124" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>